<commit_message>
Upload of input data with citations
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnorton/Models/SCOPE/SCOPE_v1.73/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoe_pierrat/Documents/GitHub/SCOPE_matlab/SCOPE_v1.73/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD2DCC6-D30C-F84E-B355-06822214AF43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243B39CC-0EE6-2142-8A53-EA7523402FF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21400" yWindow="-4080" windowWidth="21400" windowHeight="20860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -3127,7 +3127,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3349,7 +3349,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
         <v>344</v>

</xml_diff>

<commit_message>
Updates to input data and citations with OBS data, update the git ignore file to ignore output
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoe_pierrat/Documents/GitHub/SCOPE_matlab/SCOPE_v1.73/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243B39CC-0EE6-2142-8A53-EA7523402FF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9CAF50-AC6E-F746-82D8-6A726DCA36DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21400" yWindow="-4080" windowWidth="21400" windowHeight="20860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21400" yWindow="2160" windowWidth="21400" windowHeight="14620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3126,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3582,8 +3584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:DV91"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3638,7 +3640,7 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
         <v>134</v>
@@ -3653,7 +3655,7 @@
         <v>308</v>
       </c>
       <c r="B10">
-        <v>6.25</v>
+        <v>7.8</v>
       </c>
       <c r="H10" t="s">
         <v>134</v>
@@ -3776,7 +3778,7 @@
         <v>16</v>
       </c>
       <c r="B20">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H20" t="s">
         <v>146</v>
@@ -3791,7 +3793,7 @@
         <v>17</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>2.7E-2</v>
       </c>
       <c r="I21" t="s">
         <v>148</v>
@@ -3809,7 +3811,7 @@
         <v>317</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AB22" s="9"/>
       <c r="AZ22" s="4"/>
@@ -4128,7 +4130,7 @@
         <v>99</v>
       </c>
       <c r="B44">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="I44" t="s">
         <v>162</v>
@@ -4197,8 +4199,8 @@
       <c r="A50" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="9">
-        <v>3.8</v>
+      <c r="B50">
+        <v>3.6</v>
       </c>
       <c r="H50" t="s">
         <v>163</v>
@@ -4311,7 +4313,7 @@
         <v>24</v>
       </c>
       <c r="B51">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H51" t="s">
         <v>17</v>
@@ -4514,7 +4516,8 @@
         <v>23</v>
       </c>
       <c r="B68">
-        <v>1.79</v>
+        <f>0.123*B51</f>
+        <v>1.968</v>
       </c>
       <c r="H68" t="s">
         <v>17</v>
@@ -4529,7 +4532,8 @@
         <v>25</v>
       </c>
       <c r="B69">
-        <v>7.6</v>
+        <f>0.67*B51</f>
+        <v>10.72</v>
       </c>
       <c r="H69" t="s">
         <v>17</v>
@@ -4648,8 +4652,8 @@
       <c r="A80" t="s">
         <v>52</v>
       </c>
-      <c r="B80" s="9">
-        <v>204.01</v>
+      <c r="B80">
+        <v>1</v>
       </c>
       <c r="I80" t="s">
         <v>194</v>
@@ -4661,7 +4665,7 @@
         <v>53</v>
       </c>
       <c r="B81">
-        <v>204.99</v>
+        <v>365</v>
       </c>
       <c r="I81" t="s">
         <v>195</v>
@@ -4688,7 +4692,7 @@
         <v>79</v>
       </c>
       <c r="B83">
-        <v>254.88</v>
+        <v>105.12</v>
       </c>
       <c r="H83" t="s">
         <v>196</v>
@@ -4722,7 +4726,7 @@
       <c r="A87" t="s">
         <v>96</v>
       </c>
-      <c r="B87" s="9">
+      <c r="B87">
         <v>45</v>
       </c>
       <c r="H87" t="s">
@@ -4737,7 +4741,7 @@
       <c r="A88" t="s">
         <v>97</v>
       </c>
-      <c r="B88" s="9">
+      <c r="B88">
         <v>0</v>
       </c>
       <c r="H88" t="s">
@@ -4752,7 +4756,7 @@
       <c r="A89" t="s">
         <v>98</v>
       </c>
-      <c r="B89" s="9">
+      <c r="B89">
         <v>90</v>
       </c>
       <c r="H89" t="s">
@@ -4767,7 +4771,7 @@
       <c r="A90" t="s">
         <v>345</v>
       </c>
-      <c r="B90" s="9">
+      <c r="B90">
         <v>180</v>
       </c>
       <c r="H90" t="s">
@@ -4781,7 +4785,7 @@
       <c r="A91" t="s">
         <v>349</v>
       </c>
-      <c r="B91" s="9">
+      <c r="B91">
         <v>0</v>
       </c>
       <c r="H91" t="s">

</xml_diff>

<commit_message>
Edits to Input data
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoe_pierrat/Documents/GitHub/SCOPE_matlab/SCOPE_v1.73/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9CAF50-AC6E-F746-82D8-6A726DCA36DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7252DD-8EAB-694C-9852-8BE1D3D36D0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21400" yWindow="2160" windowWidth="21400" windowHeight="14620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29440" yWindow="-2320" windowWidth="15840" windowHeight="19800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="352">
   <si>
     <t>Cab</t>
   </si>
@@ -1175,13 +1175,7 @@
     <t>ta_.dat</t>
   </si>
   <si>
-    <t>lai_constant_.dat</t>
-  </si>
-  <si>
     <t>CA-OBS-2019</t>
-  </si>
-  <si>
-    <t>FLEX-S3_std.atm</t>
   </si>
   <si>
     <t>calculate the azimuthal difference between solar and observation angle (psi) according to a fixed observation azimuth angle (i.e. psi varies according to the sun-sensor geometry)</t>
@@ -1248,6 +1242,15 @@
   </si>
   <si>
     <t>solar azimuth angle</t>
+  </si>
+  <si>
+    <t>RaymentTreePhys2002_vcmax_.dat</t>
+  </si>
+  <si>
+    <t>CA-OBS-2019_Diffuse</t>
+  </si>
+  <si>
+    <t>FLEX-S3_V05.atm</t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J96"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3129,7 +3132,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:F23"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3346,7 +3349,7 @@
         <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -3354,10 +3357,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -3371,14 +3374,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
@@ -3398,7 +3401,7 @@
         <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3422,7 +3425,7 @@
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3435,7 +3438,7 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3541,9 +3544,6 @@
       <c r="A29" t="s">
         <v>68</v>
       </c>
-      <c r="B29" t="s">
-        <v>340</v>
-      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -3553,6 +3553,9 @@
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>71</v>
+      </c>
+      <c r="B31" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -3584,8 +3587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:DV91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4653,7 +4656,7 @@
         <v>52</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="I80" t="s">
         <v>194</v>
@@ -4665,7 +4668,7 @@
         <v>53</v>
       </c>
       <c r="B81">
-        <v>365</v>
+        <v>245</v>
       </c>
       <c r="I81" t="s">
         <v>195</v>
@@ -4677,7 +4680,7 @@
         <v>78</v>
       </c>
       <c r="B82">
-        <v>53.98</v>
+        <v>53.987000000000002</v>
       </c>
       <c r="H82" t="s">
         <v>196</v>
@@ -4692,7 +4695,7 @@
         <v>79</v>
       </c>
       <c r="B83">
-        <v>105.12</v>
+        <v>254.88300000000001</v>
       </c>
       <c r="H83" t="s">
         <v>196</v>
@@ -4727,7 +4730,7 @@
         <v>96</v>
       </c>
       <c r="B87">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H87" t="s">
         <v>201</v>
@@ -4763,13 +4766,13 @@
         <v>201</v>
       </c>
       <c r="I89" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AB89" s="9"/>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B90">
         <v>180</v>
@@ -4778,21 +4781,21 @@
         <v>201</v>
       </c>
       <c r="I90" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>-40</v>
       </c>
       <c r="H91" t="s">
         <v>201</v>
       </c>
       <c r="I91" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>